<commit_message>
updated with 50 more movies
</commit_message>
<xml_diff>
--- a/Data Wrangling Project.xlsx
+++ b/Data Wrangling Project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R Development\DW Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737635ED-E574-4301-8781-B2BB7DBC064F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C272E3E-6F2B-453F-9F66-4F86E9263859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="2160" windowWidth="19200" windowHeight="9970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="182">
   <si>
     <t>Inside Out 2</t>
   </si>
@@ -298,7 +298,274 @@
     <t>link</t>
   </si>
   <si>
-    <t>rottentomato</t>
+    <t>Reagan</t>
+  </si>
+  <si>
+    <t>The Forge</t>
+  </si>
+  <si>
+    <t>Horizon: An American Saga - Chapter 1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=YYsReoZMj1k</t>
+  </si>
+  <si>
+    <t>A Complete Unknown</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=FdV-Cs5o8mc</t>
+  </si>
+  <si>
+    <t>Imaginary</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=8XoNfrgrAGM</t>
+  </si>
+  <si>
+    <t>Heretic</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=O9i2vmFhSSY</t>
+  </si>
+  <si>
+    <t>Abigail</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=3PsP8MFH8p0</t>
+  </si>
+  <si>
+    <t>Monkey Man</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=g8zxiB5Qhsc</t>
+  </si>
+  <si>
+    <t>Arthur the King</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=wjDJNEPghNY</t>
+  </si>
+  <si>
+    <t>We Live in Time</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=bS0Clau5700</t>
+  </si>
+  <si>
+    <t>Poor Things</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=_klfx5sGzFk</t>
+  </si>
+  <si>
+    <t>Blink Twice</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=aMcmfonGWY4</t>
+  </si>
+  <si>
+    <t>Kraven the Hunter</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=I8gFw4-2RBM</t>
+  </si>
+  <si>
+    <t>The Bikeriders</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=BrSaVt5pvPk</t>
+  </si>
+  <si>
+    <t>The Ministry of Ungentlemanly Warfare</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=zvwDen1Wrx8</t>
+  </si>
+  <si>
+    <t>Fly Me to the Moon</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=lW7enw6mFxs</t>
+  </si>
+  <si>
+    <t>Unsung Hero</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=UHyrHRNX9Rk</t>
+  </si>
+  <si>
+    <t>The First Omen</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=lmN1Op8ygno</t>
+  </si>
+  <si>
+    <t>Cabrini</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ZaMlUazXvyY</t>
+  </si>
+  <si>
+    <t>American Fiction</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=i0MbLCpYJPA</t>
+  </si>
+  <si>
+    <t>Ordinary Angels</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=R1vn8kPgCYA</t>
+  </si>
+  <si>
+    <t>The Iron Claw</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=8KVsaoveTbw</t>
+  </si>
+  <si>
+    <t>The Watchers</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=dYo91Fq9tKY</t>
+  </si>
+  <si>
+    <t>Tarot</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=bvDArsKoTOE</t>
+  </si>
+  <si>
+    <t>Demon Slayer: Kimetsu No Yaiba - To the Hashira Training</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=SXcCdQdcBtw</t>
+  </si>
+  <si>
+    <t>Harold and the Purple Crayon</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=WojIv-PVYm8</t>
+  </si>
+  <si>
+    <t>The Color Purple</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=wPwzBUui1GA</t>
+  </si>
+  <si>
+    <t>The Substance</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=LNlrGhBpYjc</t>
+  </si>
+  <si>
+    <t>Immaculate</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=MACU-2pqVOI</t>
+  </si>
+  <si>
+    <t>Borderlands</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=lU_NKNZljoQ</t>
+  </si>
+  <si>
+    <t>MaXXXine</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=y0uS3t6nFgY</t>
+  </si>
+  <si>
+    <t>Anora</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=GuPkfvxmtdw</t>
+  </si>
+  <si>
+    <t>Homestead</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=XURLw2XXHWA</t>
+  </si>
+  <si>
+    <t>Kalki 2898 AD</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=y1-w1kUGuz8</t>
+  </si>
+  <si>
+    <t>Am I Racist?</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=c7PA_kshZh0</t>
+  </si>
+  <si>
+    <t>Here</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=I_id-SkGU2k</t>
+  </si>
+  <si>
+    <t>Bonhoeffer</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=WZM90izJ8sI</t>
+  </si>
+  <si>
+    <t>Sound of Hope: The Story of Possum Trot</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=-nyh9tcGFcI</t>
+  </si>
+  <si>
+    <t>Godzilla Minus One</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=r7DqccP1Q_4</t>
+  </si>
+  <si>
+    <t>The Boy and the Heron</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=t5khm-VjEu4</t>
+  </si>
+  <si>
+    <t>Never Let Go</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ZDfRp_ukHDU</t>
+  </si>
+  <si>
+    <t>Late Night with the Devil</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=cvt-mauboTc</t>
+  </si>
+  <si>
+    <t>Lisa Frankenstein</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=POOeA3zCuUY</t>
+  </si>
+  <si>
+    <t>Piece by Piece</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=7Bc6trBc1kc</t>
+  </si>
+  <si>
+    <t>Saturday Night</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=iZ9O_tl5Npk</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=J_vdTwQP1a8</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=HjssF55F05I</t>
   </si>
 </sst>
 </file>
@@ -313,16 +580,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="10"/>
-      <color theme="1"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="10"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -333,7 +602,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -341,16 +610,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -567,572 +857,837 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:B91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C8">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C9">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C10">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C11">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C12">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C13">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C14">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C15">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C16">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C17">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C18">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C19">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C20">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C21">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C22">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C23">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C24">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C25">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C26">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C27">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C28">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:2" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C29">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C30">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C31">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C32">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C33">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C34">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C35">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C36">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:2" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C37">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C38">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C39">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C40">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:2" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C41">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C42">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:2" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C43">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C44">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C45">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C46">
+    </row>
+    <row r="47" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="12.5" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:3" ht="12.5" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="12.5" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="12.5" x14ac:dyDescent="0.25"/>
+      <c r="B50" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
-    <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="B12" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
-    <hyperlink ref="B13" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="B14" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
-    <hyperlink ref="B15" r:id="rId14" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="B16" r:id="rId15" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
-    <hyperlink ref="B17" r:id="rId16" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
-    <hyperlink ref="B18" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
-    <hyperlink ref="B19" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink ref="B20" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
-    <hyperlink ref="B21" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
-    <hyperlink ref="B22" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
-    <hyperlink ref="B23" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink ref="B24" r:id="rId23" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
-    <hyperlink ref="B25" r:id="rId24" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
-    <hyperlink ref="B26" r:id="rId25" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
-    <hyperlink ref="B27" r:id="rId26" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="B28" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
-    <hyperlink ref="B29" r:id="rId28" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink ref="B30" r:id="rId29" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
-    <hyperlink ref="B31" r:id="rId30" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink ref="B32" r:id="rId31" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
-    <hyperlink ref="B33" r:id="rId32" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
-    <hyperlink ref="B34" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
-    <hyperlink ref="B35" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
-    <hyperlink ref="B36" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
-    <hyperlink ref="B37" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
-    <hyperlink ref="B38" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
-    <hyperlink ref="B39" r:id="rId38" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
-    <hyperlink ref="B40" r:id="rId39" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
-    <hyperlink ref="B41" r:id="rId40" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
-    <hyperlink ref="B42" r:id="rId41" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
-    <hyperlink ref="B43" r:id="rId42" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
-    <hyperlink ref="B44" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
-    <hyperlink ref="B45" r:id="rId44" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
-    <hyperlink ref="B46" r:id="rId45" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{1222C887-8908-47B3-9C9E-276ADA47D07A}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{4230BFC4-7206-4A93-AC12-2261CEE2AE64}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{8B56ECB7-18C7-49FE-AE4A-C3493EBDE35B}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{F9797769-4A95-4CD9-9C64-D14C2AC09945}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{922ABE57-2D5D-4E83-A71F-B0E0FB57AC83}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{B5B39DA9-AAFB-40C3-92B3-294DD960D8AE}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{8942D2C3-09E8-48C0-A66C-638234B7D36A}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{A8A1CCB8-A5DB-4E55-B1A5-9A862DD9100D}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{47B56A12-CC13-41BF-BA08-2684064303F2}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{7714A16E-D9FF-4680-B626-796B30031F1D}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{98BE81EB-AD3E-47A1-957D-85F7E3D4D34C}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{0FEC0071-A5A6-42FA-9BAE-2E939CA970B8}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{D3841D40-DE0D-485D-910E-AAA012070D97}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{696EC455-0BA9-42E5-AF3F-AAB54B1B0F1D}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{A8B22C6C-60EE-4A73-8782-F4C91DDD447A}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{794D821A-5A1F-4C26-AF59-79B7CE33C8B2}"/>
+    <hyperlink ref="B18" r:id="rId17" xr:uid="{6CB4FCB1-BD5E-4DD6-A33C-EC4AA0759CEA}"/>
+    <hyperlink ref="B19" r:id="rId18" xr:uid="{CB2B126E-85E2-4C67-B45C-35B2FFEB6263}"/>
+    <hyperlink ref="B20" r:id="rId19" xr:uid="{34321174-D7F5-4F2A-B043-CE613C052066}"/>
+    <hyperlink ref="B21" r:id="rId20" xr:uid="{BD26B62B-7A43-405A-BFCA-1075CBD592F0}"/>
+    <hyperlink ref="B22" r:id="rId21" xr:uid="{7FF1DB35-5AC0-4F98-9320-46DA097C0FF1}"/>
+    <hyperlink ref="B23" r:id="rId22" xr:uid="{3941A93A-1C8C-4B34-A174-BAE7A4A8A300}"/>
+    <hyperlink ref="B24" r:id="rId23" xr:uid="{516F9AC3-7536-495A-A07E-F94A81D7CA20}"/>
+    <hyperlink ref="B25" r:id="rId24" xr:uid="{51961298-2044-4523-A28A-E16C441E069F}"/>
+    <hyperlink ref="B26" r:id="rId25" xr:uid="{88EE794B-D64D-455F-8C22-14F7AF0F8582}"/>
+    <hyperlink ref="B27" r:id="rId26" xr:uid="{3DB14401-D306-448C-9567-956792BF7DD1}"/>
+    <hyperlink ref="B28" r:id="rId27" xr:uid="{21050B04-FCA3-4B53-8EED-2DDE4E4A837B}"/>
+    <hyperlink ref="B29" r:id="rId28" xr:uid="{EF2626A3-6ABA-4D9D-B261-3354E8F7AE43}"/>
+    <hyperlink ref="B30" r:id="rId29" xr:uid="{0F829859-10A2-4F96-85A0-3B42936855BA}"/>
+    <hyperlink ref="B31" r:id="rId30" xr:uid="{FB18DA90-2196-4288-A41B-40A7F02B0336}"/>
+    <hyperlink ref="B32" r:id="rId31" xr:uid="{8254899C-DEBA-4286-B914-3E95304ED084}"/>
+    <hyperlink ref="B33" r:id="rId32" xr:uid="{51B68C22-7408-4DE7-9DA0-6BE3B13386C9}"/>
+    <hyperlink ref="B34" r:id="rId33" xr:uid="{7EEF3A8F-2E17-438F-8223-9F6DE94018E5}"/>
+    <hyperlink ref="B35" r:id="rId34" xr:uid="{3C3C991C-AF33-44BE-82E9-10E7655C4B85}"/>
+    <hyperlink ref="B36" r:id="rId35" xr:uid="{A8A73CEC-7C95-4E45-A921-EE509D24507D}"/>
+    <hyperlink ref="B37" r:id="rId36" xr:uid="{0C103C9B-86AF-486C-B701-95B2A5953EC8}"/>
+    <hyperlink ref="B38" r:id="rId37" xr:uid="{2A3633D8-29DB-4664-988C-5D1567A00C53}"/>
+    <hyperlink ref="B39" r:id="rId38" xr:uid="{010BB7CC-1AFE-404E-85E2-51089B375534}"/>
+    <hyperlink ref="B40" r:id="rId39" xr:uid="{73A2E104-40D0-4270-9898-18BA3B00528D}"/>
+    <hyperlink ref="B41" r:id="rId40" xr:uid="{F90270E5-C424-4E23-81AD-403798C38877}"/>
+    <hyperlink ref="B42" r:id="rId41" xr:uid="{181B0E97-F02C-47B9-808C-FEF2851DC3D7}"/>
+    <hyperlink ref="B43" r:id="rId42" xr:uid="{F8C294CD-993C-4457-88EC-918497C4263F}"/>
+    <hyperlink ref="B44" r:id="rId43" xr:uid="{3D126127-C5BE-4D09-9B0F-5AFBA90BDB14}"/>
+    <hyperlink ref="B45" r:id="rId44" xr:uid="{F88FAC7C-6140-42D5-B85D-9412EE840AE4}"/>
+    <hyperlink ref="B46" r:id="rId45" xr:uid="{034E0DF1-448B-4A85-8C81-FA8CA3C13A5C}"/>
+    <hyperlink ref="B49" r:id="rId46" xr:uid="{917A7EFE-6A66-4507-B6A5-A81829DBCDF1}"/>
+    <hyperlink ref="B50" r:id="rId47" xr:uid="{3DBB72DB-557A-4822-BA83-67C7AC074341}"/>
+    <hyperlink ref="B51" r:id="rId48" xr:uid="{B28664DA-43B5-4D6E-9586-557F2A5CE0A1}"/>
+    <hyperlink ref="B52" r:id="rId49" xr:uid="{57C153F8-8B36-4822-AFD5-55D1ABAB8F6D}"/>
+    <hyperlink ref="B53" r:id="rId50" xr:uid="{7E258467-FD1A-42E9-BFF0-5EB94EE285F1}"/>
+    <hyperlink ref="B54" r:id="rId51" xr:uid="{D4435614-7D90-4963-8754-4A036021BF4A}"/>
+    <hyperlink ref="B55" r:id="rId52" xr:uid="{9C30EF54-1673-4278-91D1-2033F4F95F68}"/>
+    <hyperlink ref="B56" r:id="rId53" xr:uid="{663E1597-09CA-4F25-9CD9-6154EED9F6BD}"/>
+    <hyperlink ref="B57" r:id="rId54" xr:uid="{B698ABDD-A314-4E94-B347-BFDD6FEBA949}"/>
+    <hyperlink ref="B58" r:id="rId55" xr:uid="{9FA22764-E1DA-4C72-BFFB-10086CDC5643}"/>
+    <hyperlink ref="B59" r:id="rId56" xr:uid="{96FF4F42-BB4F-41BD-BEB2-8EFBBB372F54}"/>
+    <hyperlink ref="B60" r:id="rId57" xr:uid="{84C8B6FE-E9EC-4EFE-AA63-3EF610016674}"/>
+    <hyperlink ref="B61" r:id="rId58" xr:uid="{6CDCEA14-93CD-48D1-84E8-DAB065537AC1}"/>
+    <hyperlink ref="B62" r:id="rId59" xr:uid="{5F5CE16C-E8D6-4825-96F0-A3D13D717E66}"/>
+    <hyperlink ref="B63" r:id="rId60" xr:uid="{50DD9439-1725-4232-93BA-00E3F326D0EA}"/>
+    <hyperlink ref="B64" r:id="rId61" xr:uid="{2EDDEF70-2593-4207-A006-67FB0B49DD61}"/>
+    <hyperlink ref="B65" r:id="rId62" xr:uid="{318A5DB6-5774-4F1F-943B-373C7477FE8D}"/>
+    <hyperlink ref="B66" r:id="rId63" xr:uid="{426FAEDD-1516-4494-85EA-A58B9F4210E9}"/>
+    <hyperlink ref="B67" r:id="rId64" xr:uid="{D6472C9A-BC45-438A-9813-8F19D63D5290}"/>
+    <hyperlink ref="B68" r:id="rId65" xr:uid="{11DDBC0F-D4E0-4D1C-89C0-448FCD4BD18F}"/>
+    <hyperlink ref="B69" r:id="rId66" xr:uid="{4C908D4E-9E38-45E2-B151-BB2AC3B7ABE5}"/>
+    <hyperlink ref="B70" r:id="rId67" xr:uid="{1443155D-4953-4BA6-8578-F8644736DF65}"/>
+    <hyperlink ref="B71" r:id="rId68" xr:uid="{13D61364-095C-4B44-9AB0-0F7C48FAF539}"/>
+    <hyperlink ref="B72" r:id="rId69" xr:uid="{6C0ABBC0-68B4-4EEA-AD9F-1D390D86C3ED}"/>
+    <hyperlink ref="B73" r:id="rId70" xr:uid="{E06983A1-35FB-4EC6-8F47-FCFC33B1CC0A}"/>
+    <hyperlink ref="B74" r:id="rId71" xr:uid="{CA6B6980-88DD-485D-B0FC-DD661613822E}"/>
+    <hyperlink ref="B75" r:id="rId72" xr:uid="{81F33F04-25DF-4A4F-B35F-72582846C892}"/>
+    <hyperlink ref="B76" r:id="rId73" xr:uid="{AE340E90-E4F9-47FA-94DD-801C18835FA5}"/>
+    <hyperlink ref="B77" r:id="rId74" xr:uid="{9D3FA4E7-B1E2-40B8-83CC-5368B75639E9}"/>
+    <hyperlink ref="B78" r:id="rId75" xr:uid="{161D84B2-E67B-42BA-A98C-910F560B4CDF}"/>
+    <hyperlink ref="B79" r:id="rId76" xr:uid="{47F09620-CEE5-432B-8627-7DBA908C235E}"/>
+    <hyperlink ref="B80" r:id="rId77" xr:uid="{50663E29-CB73-4F31-8899-92D10299B2F2}"/>
+    <hyperlink ref="B81" r:id="rId78" xr:uid="{DBD0061A-1250-4DAB-9C7D-63CCDE0A1FFB}"/>
+    <hyperlink ref="B82" r:id="rId79" xr:uid="{5F492B1B-7E67-4E73-AD3C-08C511C8FB14}"/>
+    <hyperlink ref="B83" r:id="rId80" xr:uid="{54C680CD-99FF-4F78-B218-BEA4FE2BBB5A}"/>
+    <hyperlink ref="B84" r:id="rId81" xr:uid="{E489D036-15B8-4B49-8EF9-9117511E314D}"/>
+    <hyperlink ref="B85" r:id="rId82" xr:uid="{E33970DB-BB0F-4A08-A1CF-674207AF7B1F}"/>
+    <hyperlink ref="B86" r:id="rId83" xr:uid="{359FFBFF-423F-4F43-BC5F-41AEAB2B90A9}"/>
+    <hyperlink ref="B87" r:id="rId84" xr:uid="{116CE658-411E-4FDE-B1EE-FB329539B0E3}"/>
+    <hyperlink ref="B88" r:id="rId85" xr:uid="{4681F206-FC2A-49AF-9F06-DA52BADF0263}"/>
+    <hyperlink ref="B89" r:id="rId86" xr:uid="{F670C94A-9649-4528-8486-C3D61097D2C7}"/>
+    <hyperlink ref="B90" r:id="rId87" xr:uid="{42F617EF-2B8B-4A6C-9FBE-12E06298C346}"/>
+    <hyperlink ref="B91" r:id="rId88" xr:uid="{09AC758D-161D-402D-87A5-857D9BD19DAE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId89"/>
 </worksheet>
 </file>
</xml_diff>